<commit_message>
Setting up the database
</commit_message>
<xml_diff>
--- a/EmissionValues.xlsx
+++ b/EmissionValues.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$46</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Almond milk</t>
   </si>
@@ -175,19 +175,10 @@
     <t>Barley</t>
   </si>
   <si>
-    <t>Kg of CO2 equivalent per Kg of Product</t>
-  </si>
-  <si>
     <t>Energy Consumption</t>
   </si>
   <si>
     <t>Water Usage</t>
-  </si>
-  <si>
-    <t>M^3 per Kg of Product</t>
-  </si>
-  <si>
-    <t>MJ per Kg of Product</t>
   </si>
   <si>
     <t>Global Warming Potential (GWP)</t>
@@ -273,7 +264,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -283,9 +274,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -604,9 +592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -617,612 +607,600 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>48</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1.0898783206332101</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.0898783206332101</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.0898783206332101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1.0898783206332101</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1.0898783206332101</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1.0898783206332101</v>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2.1797566412664202</v>
+      </c>
+      <c r="C3" s="6">
+        <v>26.309886088216</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.9013045715911601</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2.1797566412664202</v>
-      </c>
-      <c r="C4" s="7">
-        <v>26.309886088216</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1.9013045715911601</v>
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>27.759977591671198</v>
+      </c>
+      <c r="C4" s="6">
+        <v>164.224859803377</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.469425987022143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>27.759977591671198</v>
-      </c>
-      <c r="C5" s="7">
-        <v>164.224859803377</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.469425987022143</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>8.2898653954866894</v>
+      </c>
+      <c r="C5" s="6">
+        <v>35.495578261973101</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.14570166801345499</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7">
-        <v>8.2898653954866894</v>
-      </c>
-      <c r="C6" s="7">
-        <v>35.495578261973101</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.14570166801345499</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>6.2027222398178896</v>
+      </c>
+      <c r="C6" s="6">
+        <v>26.705441762149601</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.108737614894822</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7">
-        <v>6.2027222398178896</v>
-      </c>
-      <c r="C7" s="7">
-        <v>26.705441762149601</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0.108737614894822</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6.8188280359115296</v>
+      </c>
+      <c r="C7" s="6">
+        <v>64.135317267657001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.33902140273791398</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7">
-        <v>6.8188280359115296</v>
-      </c>
-      <c r="C8" s="7">
-        <v>64.135317267657001</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.33902140273791398</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>14.6743296898354</v>
+      </c>
+      <c r="C8" s="6">
+        <v>90.248969315788102</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.37513623312745797</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7">
-        <v>14.6743296898354</v>
-      </c>
-      <c r="C9" s="7">
-        <v>90.248969315788102</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.37513623312745797</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>4.6525659491155826</v>
+      </c>
+      <c r="C9" s="6">
+        <v>26.923822947676342</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.11053844368761952</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7">
-        <v>4.6525659491155826</v>
-      </c>
-      <c r="C10" s="7">
-        <v>26.923822947676342</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.11053844368761952</v>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.19045655136876699</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.8766423371080601</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5.725737294377E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.19045655136876699</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1.8766423371080601</v>
-      </c>
-      <c r="D11" s="7">
-        <v>5.725737294377E-2</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>27.759977591671198</v>
+      </c>
+      <c r="C11" s="6">
+        <v>164.224859803377</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.469425987022143</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7">
-        <v>27.759977591671198</v>
-      </c>
-      <c r="C12" s="7">
-        <v>164.224859803377</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.469425987022143</v>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.4931742795549099</v>
+      </c>
+      <c r="C12" s="6">
+        <v>17.225670324435601</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.18891713900774E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1.4931742795549099</v>
-      </c>
-      <c r="C13" s="7">
-        <v>17.225670324435601</v>
-      </c>
-      <c r="D13" s="7">
-        <v>1.18891713900774E-2</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>10.247750506055313</v>
+      </c>
+      <c r="C13" s="6">
+        <v>66.218777610734321</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.16438500312310583</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7">
-        <v>10.247750506055313</v>
-      </c>
-      <c r="C14" s="7">
-        <v>66.218777610734321</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.16438500312310583</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3.0627172972826053</v>
+      </c>
+      <c r="C14" s="6">
+        <v>20.383555577593235</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4.4167568693069773E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7">
-        <v>3.0627172972826053</v>
-      </c>
-      <c r="C15" s="7">
-        <v>20.383555577593235</v>
-      </c>
-      <c r="D15" s="7">
-        <v>4.4167568693069773E-2</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>8.2898653954866894</v>
+      </c>
+      <c r="C15" s="6">
+        <v>35.495578261973101</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.14570166801345499</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7">
-        <v>8.2898653954866894</v>
-      </c>
-      <c r="C16" s="7">
-        <v>35.495578261973101</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.14570166801345499</v>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>10.761064044114701</v>
+      </c>
+      <c r="C16" s="6">
+        <v>91.401807604847093</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.52107065489710402</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7">
-        <v>10.761064044114701</v>
-      </c>
-      <c r="C17" s="7">
-        <v>91.401807604847093</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.52107065489710402</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.78396357243263803</v>
+      </c>
+      <c r="C17" s="6">
+        <v>5.67374478926682</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.13569536742406299</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7">
-        <v>0.78396357243263803</v>
-      </c>
-      <c r="C18" s="7">
-        <v>5.67374478926682</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0.13569536742406299</v>
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.10754569554789</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1.3893857124698801</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.4149503710495399E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1.10754569554789</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1.3893857124698801</v>
-      </c>
-      <c r="D19" s="7">
-        <v>1.4149503710495399E-3</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>3.94395544753558</v>
+      </c>
+      <c r="C19" s="6">
+        <v>36.099327234101899</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.18456657454426301</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7">
-        <v>3.94395544753558</v>
-      </c>
-      <c r="C20" s="7">
-        <v>36.099327234101899</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0.18456657454426301</v>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>10.761064044114701</v>
+      </c>
+      <c r="C20" s="6">
+        <v>91.401807604847093</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.52107065489710402</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
         <v>10.761064044114701</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>91.401807604847093</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>0.52107065489710402</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
         <v>10.761064044114701</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>91.401807604847093</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>0.52107065489710402</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="7">
-        <v>10.761064044114701</v>
-      </c>
-      <c r="C23" s="7">
-        <v>91.401807604847093</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.52107065489710402</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.19045655136876699</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1.8766423371080601</v>
+      </c>
+      <c r="D23" s="6">
+        <v>5.725737294377E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="7">
-        <v>0.19045655136876699</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1.8766423371080601</v>
-      </c>
-      <c r="D24" s="7">
-        <v>5.725737294377E-2</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.78396357243263803</v>
+      </c>
+      <c r="C24" s="6">
+        <v>5.67374478926682</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.13569536742406299</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="7">
-        <v>0.78396357243263803</v>
-      </c>
-      <c r="C25" s="7">
-        <v>5.67374478926682</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.13569536742406299</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.25712987138015753</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.25712987138015753</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.25712987138015753</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="7">
-        <v>0.25712987138015753</v>
-      </c>
-      <c r="C26" s="7">
-        <v>0.25712987138015753</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.25712987138015753</v>
+      <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1.0285194855206301</v>
+      </c>
+      <c r="C26" s="6">
+        <v>5.4292410453906701</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.35153526300458998</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="7">
-        <v>1.0285194855206301</v>
-      </c>
-      <c r="C27" s="7">
-        <v>5.4292410453906701</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0.35153526300458998</v>
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6">
+        <v>27.759977591671198</v>
+      </c>
+      <c r="C27" s="6">
+        <v>164.224859803377</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.469425987022143</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7">
-        <v>27.759977591671198</v>
-      </c>
-      <c r="C28" s="7">
-        <v>164.224859803377</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0.469425987022143</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="C28" s="4">
+        <v>64</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.34</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4">
-        <v>6.8</v>
-      </c>
-      <c r="C29" s="4">
-        <v>64</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.34</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <v>6.2027222398178896</v>
+      </c>
+      <c r="C29" s="6">
+        <v>26.705441762149601</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.108737614894822</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="7">
-        <v>6.2027222398178896</v>
-      </c>
-      <c r="C30" s="7">
-        <v>26.705441762149601</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0.108737614894822</v>
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6">
+        <v>3.4404711732447097</v>
+      </c>
+      <c r="C30" s="6">
+        <v>28.522439195720203</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.10953513289494721</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7">
-        <v>3.4404711732447097</v>
-      </c>
-      <c r="C31" s="7">
-        <v>28.522439195720203</v>
-      </c>
-      <c r="D31" s="7">
-        <v>0.10953513289494721</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="6">
+        <v>3.2321245133174301</v>
+      </c>
+      <c r="C31" s="6">
+        <v>14.366381167705001</v>
+      </c>
+      <c r="D31" s="6">
+        <v>4.2499828861568096E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7">
-        <v>3.2321245133174301</v>
-      </c>
-      <c r="C32" s="7">
-        <v>14.366381167705001</v>
-      </c>
-      <c r="D32" s="7">
-        <v>4.2499828861568096E-3</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1.3119780355423101</v>
+      </c>
+      <c r="C32" s="6">
+        <v>5.8154408249724199</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2.2339180541006701E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7">
-        <v>1.3119780355423101</v>
-      </c>
-      <c r="C33" s="7">
-        <v>5.8154408249724199</v>
-      </c>
-      <c r="D33" s="7">
-        <v>2.2339180541006701E-2</v>
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.19045655136876699</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1.8766423371080601</v>
+      </c>
+      <c r="D33" s="6">
+        <v>5.725737294377E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="7">
-        <v>0.19045655136876699</v>
-      </c>
-      <c r="C34" s="7">
-        <v>1.8766423371080601</v>
-      </c>
-      <c r="D34" s="7">
-        <v>5.725737294377E-2</v>
+      <c r="A34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1.4931742795549099</v>
+      </c>
+      <c r="C34" s="6">
+        <v>17.225670324435601</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.18891713900774E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1.4931742795549099</v>
-      </c>
-      <c r="C35" s="7">
-        <v>17.225670324435601</v>
-      </c>
-      <c r="D35" s="7">
-        <v>1.18891713900774E-2</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B35" s="4">
+        <v>25.44</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>25.44</v>
+        <v>11.52</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4">
-        <v>11.52</v>
+        <v>5.9</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4">
-        <v>5.9</v>
+        <v>3.61</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>3.61</v>
+        <v>3.49</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="4">
-        <v>3.49</v>
+        <v>3.4</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4">
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4">
-        <v>2.2999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="4">
-        <v>0.6</v>
+        <v>0.52</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B46" s="4">
-        <v>0.52</v>
+        <v>0.67</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="4">
-        <v>0.67</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>